<commit_message>
final presentation version, added initial final_report
</commit_message>
<xml_diff>
--- a/deliverables/presentation/nathan/timings_AB.xlsx
+++ b/deliverables/presentation/nathan/timings_AB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,8 +112,24 @@
       <color theme="1"/>
       <name val="Calibri Light"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,8 +166,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -160,7 +182,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -178,7 +200,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thick">
@@ -190,13 +212,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -205,7 +227,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -223,7 +245,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thick">
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
@@ -235,6 +257,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thick">
         <color auto="1"/>
       </left>
@@ -416,8 +453,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -426,110 +465,112 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -859,198 +900,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P19"/>
+  <dimension ref="C2:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="39.83203125" style="2" customWidth="1"/>
-    <col min="4" max="13" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="18.33203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="18.5" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="1.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="39.83203125" style="2" customWidth="1"/>
+    <col min="5" max="14" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18.5" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="3:17" ht="25">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="16" thickBot="1"/>
-    <row r="4" spans="2:16" ht="33" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B4" s="27" t="s">
+    <row r="3" spans="3:17" ht="16" thickBot="1"/>
+    <row r="4" spans="3:17" ht="33" customHeight="1" thickTop="1" thickBot="1">
+      <c r="C4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="D4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="28">
+      <c r="E4" s="25">
         <v>1</v>
       </c>
-      <c r="E4" s="28">
+      <c r="F4" s="25">
         <v>2</v>
       </c>
-      <c r="F4" s="28">
+      <c r="G4" s="25">
         <v>3</v>
       </c>
-      <c r="G4" s="28">
+      <c r="H4" s="25">
         <v>4</v>
       </c>
-      <c r="H4" s="28">
+      <c r="I4" s="25">
         <v>5</v>
       </c>
-      <c r="I4" s="28">
+      <c r="J4" s="25">
         <v>6</v>
       </c>
-      <c r="J4" s="28">
+      <c r="K4" s="25">
         <v>7</v>
       </c>
-      <c r="K4" s="28">
+      <c r="L4" s="25">
         <v>8</v>
       </c>
-      <c r="L4" s="28">
+      <c r="M4" s="25">
         <v>9</v>
       </c>
-      <c r="M4" s="28">
+      <c r="N4" s="25">
         <v>10</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="O4" s="26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="18" customHeight="1" thickTop="1">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="3:17" ht="18" customHeight="1" thickTop="1">
+      <c r="C5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="11">
+      <c r="E5" s="36">
         <v>8745</v>
       </c>
-      <c r="E5" s="11">
+      <c r="F5" s="36">
         <v>8758</v>
       </c>
-      <c r="F5" s="11">
+      <c r="G5" s="36">
         <v>8826</v>
       </c>
-      <c r="G5" s="11">
+      <c r="H5" s="36">
         <v>8737</v>
       </c>
-      <c r="H5" s="11">
+      <c r="I5" s="36">
         <v>8811</v>
       </c>
-      <c r="I5" s="11">
+      <c r="J5" s="36">
         <v>8728</v>
       </c>
-      <c r="J5" s="11">
+      <c r="K5" s="36">
         <v>8964</v>
       </c>
-      <c r="K5" s="11">
+      <c r="L5" s="36">
         <v>8774</v>
       </c>
-      <c r="L5" s="11">
+      <c r="M5" s="36">
         <v>8826</v>
       </c>
-      <c r="M5" s="11">
+      <c r="N5" s="36">
         <v>8787</v>
       </c>
-      <c r="N5" s="12">
-        <f>AVERAGE(D5:M5)</f>
+      <c r="O5" s="37">
+        <f>AVERAGE(E5:N5)</f>
         <v>8795.6</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="18" customHeight="1">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="3:17" ht="18" customHeight="1">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5">
+      <c r="E6" s="5">
         <v>11053</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <v>11030</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>11067</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
         <v>10988</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>11133</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>10982</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>11206</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>10985</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>10996</v>
       </c>
-      <c r="M6" s="5">
+      <c r="N6" s="5">
         <v>11002</v>
       </c>
-      <c r="N6" s="6">
-        <f t="shared" ref="N6:N18" si="0">AVERAGE(D6:M6)</f>
+      <c r="O6" s="6">
+        <f t="shared" ref="O6:O18" si="0">AVERAGE(E6:N6)</f>
         <v>11044.2</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="18" customHeight="1" thickBot="1">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="3:17" ht="18" customHeight="1" thickBot="1">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="8">
+      <c r="E7" s="8">
         <v>9944</v>
       </c>
-      <c r="E7" s="8">
+      <c r="F7" s="8">
         <v>9953</v>
       </c>
-      <c r="F7" s="8">
+      <c r="G7" s="8">
         <v>10018</v>
       </c>
-      <c r="G7" s="8">
+      <c r="H7" s="8">
         <v>10016</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="8">
         <v>10049</v>
       </c>
-      <c r="I7" s="8">
+      <c r="J7" s="8">
         <v>9937</v>
       </c>
-      <c r="J7" s="8">
+      <c r="K7" s="8">
         <v>10094</v>
       </c>
-      <c r="K7" s="8">
+      <c r="L7" s="8">
         <v>10017</v>
       </c>
-      <c r="L7" s="8">
+      <c r="M7" s="8">
         <v>10078</v>
       </c>
-      <c r="M7" s="8">
+      <c r="N7" s="8">
         <v>9966</v>
       </c>
-      <c r="N7" s="9">
+      <c r="O7" s="9">
         <f t="shared" si="0"/>
         <v>10007.200000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="16" thickTop="1">
-      <c r="B8" s="3"/>
+    <row r="8" spans="3:17" ht="16" thickTop="1">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1063,9 +1105,9 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="2:16" ht="16" thickBot="1">
-      <c r="B9" s="3"/>
+    <row r="9" spans="3:17" ht="16" thickBot="1">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1078,427 +1120,429 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="2:16" ht="17" customHeight="1" thickTop="1">
-      <c r="B10" s="21" t="s">
+    <row r="10" spans="3:17" ht="17" customHeight="1" thickTop="1">
+      <c r="C10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="D10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="23" t="s">
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="O10" s="25" t="s">
+      <c r="P10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="26"/>
+      <c r="Q10" s="23"/>
     </row>
-    <row r="11" spans="2:16" ht="16" thickBot="1">
-      <c r="B11" s="22"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="17">
+    <row r="11" spans="3:17" ht="16" thickBot="1">
+      <c r="C11" s="19"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="14">
         <v>1</v>
       </c>
-      <c r="E11" s="17">
+      <c r="F11" s="14">
         <v>2</v>
       </c>
-      <c r="F11" s="17">
+      <c r="G11" s="14">
         <v>3</v>
       </c>
-      <c r="G11" s="17">
+      <c r="H11" s="14">
         <v>4</v>
       </c>
-      <c r="H11" s="17">
+      <c r="I11" s="14">
         <v>5</v>
       </c>
-      <c r="I11" s="17">
+      <c r="J11" s="14">
         <v>6</v>
       </c>
-      <c r="J11" s="17">
+      <c r="K11" s="14">
         <v>7</v>
       </c>
-      <c r="K11" s="17">
+      <c r="L11" s="14">
         <v>8</v>
       </c>
-      <c r="L11" s="17">
+      <c r="M11" s="14">
         <v>9</v>
       </c>
-      <c r="M11" s="17">
+      <c r="N11" s="14">
         <v>10</v>
       </c>
-      <c r="N11" s="24"/>
-      <c r="O11" s="17" t="s">
+      <c r="O11" s="21"/>
+      <c r="P11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="P11" s="18" t="s">
+      <c r="Q11" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="18" customHeight="1" thickTop="1">
-      <c r="B12" s="30" t="s">
+    <row r="12" spans="3:17" ht="18" customHeight="1" thickTop="1">
+      <c r="C12" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="D12" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="31">
+      <c r="E12" s="32">
         <v>134</v>
       </c>
-      <c r="E12" s="31">
+      <c r="F12" s="32">
         <v>134</v>
       </c>
-      <c r="F12" s="31">
+      <c r="G12" s="32">
         <v>135</v>
       </c>
-      <c r="G12" s="31">
+      <c r="H12" s="32">
         <v>135</v>
       </c>
-      <c r="H12" s="31">
+      <c r="I12" s="32">
         <v>134</v>
       </c>
-      <c r="I12" s="31">
+      <c r="J12" s="32">
         <v>134</v>
       </c>
-      <c r="J12" s="31">
+      <c r="K12" s="32">
         <v>134</v>
       </c>
-      <c r="K12" s="31">
+      <c r="L12" s="32">
         <v>135</v>
       </c>
-      <c r="L12" s="31">
+      <c r="M12" s="32">
         <v>135</v>
       </c>
-      <c r="M12" s="31">
+      <c r="N12" s="32">
         <v>134</v>
       </c>
-      <c r="N12" s="32">
+      <c r="O12" s="33">
         <f t="shared" si="0"/>
         <v>134.4</v>
       </c>
-      <c r="O12" s="32">
-        <f>$N$5/N12</f>
+      <c r="P12" s="33">
+        <f>$O$5/O12</f>
         <v>65.44345238095238</v>
       </c>
-      <c r="P12" s="33">
-        <f>O12/12</f>
+      <c r="Q12" s="34">
+        <f>P12/12</f>
         <v>5.4536210317460316</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="18" customHeight="1">
-      <c r="B13" s="14" t="s">
+    <row r="13" spans="3:17" ht="18" customHeight="1">
+      <c r="C13" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="15">
+      <c r="E13" s="12">
         <v>114</v>
       </c>
-      <c r="E13" s="15">
+      <c r="F13" s="12">
         <v>115</v>
       </c>
-      <c r="F13" s="15">
+      <c r="G13" s="12">
         <v>114</v>
       </c>
-      <c r="G13" s="15">
+      <c r="H13" s="12">
         <v>114</v>
       </c>
-      <c r="H13" s="15">
+      <c r="I13" s="12">
         <v>114</v>
       </c>
-      <c r="I13" s="15">
+      <c r="J13" s="12">
         <v>114</v>
       </c>
-      <c r="J13" s="15">
+      <c r="K13" s="12">
         <v>115</v>
       </c>
-      <c r="K13" s="15">
+      <c r="L13" s="12">
         <v>114</v>
       </c>
-      <c r="L13" s="15">
+      <c r="M13" s="12">
         <v>114</v>
       </c>
-      <c r="M13" s="15">
+      <c r="N13" s="12">
         <v>114</v>
       </c>
-      <c r="N13" s="19">
+      <c r="O13" s="16">
         <f t="shared" si="0"/>
         <v>114.2</v>
       </c>
-      <c r="O13" s="19">
-        <f t="shared" ref="O13:O18" si="1">$N$5/N13</f>
+      <c r="P13" s="16">
+        <f t="shared" ref="P13:P18" si="1">$O$5/O13</f>
         <v>77.019264448336259</v>
       </c>
-      <c r="P13" s="20">
-        <f t="shared" ref="P13:P18" si="2">O13/12</f>
+      <c r="Q13" s="17">
+        <f t="shared" ref="Q13:Q18" si="2">P13/12</f>
         <v>6.4182720373613549</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="18" customHeight="1">
-      <c r="B14" s="14" t="s">
+    <row r="14" spans="3:17" ht="18" customHeight="1">
+      <c r="C14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="15">
+      <c r="D14" s="10"/>
+      <c r="E14" s="12">
         <v>114</v>
       </c>
-      <c r="E14" s="15">
+      <c r="F14" s="12">
         <v>115</v>
       </c>
-      <c r="F14" s="15">
+      <c r="G14" s="12">
         <v>114</v>
       </c>
-      <c r="G14" s="15">
+      <c r="H14" s="12">
         <v>115</v>
       </c>
-      <c r="H14" s="15">
+      <c r="I14" s="12">
         <v>114</v>
       </c>
-      <c r="I14" s="15">
+      <c r="J14" s="12">
         <v>115</v>
       </c>
-      <c r="J14" s="15">
+      <c r="K14" s="12">
         <v>115</v>
       </c>
-      <c r="K14" s="15">
+      <c r="L14" s="12">
         <v>114</v>
       </c>
-      <c r="L14" s="15">
+      <c r="M14" s="12">
         <v>114</v>
       </c>
-      <c r="M14" s="15">
+      <c r="N14" s="12">
         <v>114</v>
       </c>
-      <c r="N14" s="19">
+      <c r="O14" s="16">
         <f t="shared" si="0"/>
         <v>114.4</v>
       </c>
-      <c r="O14" s="19">
+      <c r="P14" s="16">
         <f t="shared" si="1"/>
         <v>76.884615384615387</v>
       </c>
-      <c r="P14" s="20">
+      <c r="Q14" s="17">
         <f t="shared" si="2"/>
         <v>6.4070512820512819</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="18" customHeight="1">
-      <c r="B15" s="14" t="s">
+    <row r="15" spans="3:17" ht="18" customHeight="1">
+      <c r="C15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="15">
+      <c r="D15" s="10"/>
+      <c r="E15" s="12">
         <v>113</v>
       </c>
-      <c r="E15" s="15">
+      <c r="F15" s="12">
         <v>113</v>
       </c>
-      <c r="F15" s="15">
+      <c r="G15" s="12">
         <v>112</v>
       </c>
-      <c r="G15" s="15">
+      <c r="H15" s="12">
         <v>112</v>
       </c>
-      <c r="H15" s="15">
+      <c r="I15" s="12">
         <v>111</v>
       </c>
-      <c r="I15" s="15">
+      <c r="J15" s="12">
         <v>112</v>
       </c>
-      <c r="J15" s="15">
+      <c r="K15" s="12">
         <v>112</v>
       </c>
-      <c r="K15" s="15">
+      <c r="L15" s="12">
         <v>113</v>
       </c>
-      <c r="L15" s="15">
+      <c r="M15" s="12">
         <v>112</v>
       </c>
-      <c r="M15" s="15">
+      <c r="N15" s="12">
         <v>112</v>
       </c>
-      <c r="N15" s="19">
+      <c r="O15" s="16">
         <f t="shared" si="0"/>
         <v>112.2</v>
       </c>
-      <c r="O15" s="19">
+      <c r="P15" s="16">
         <f t="shared" si="1"/>
         <v>78.392156862745097</v>
       </c>
-      <c r="P15" s="20">
+      <c r="Q15" s="17">
         <f t="shared" si="2"/>
         <v>6.5326797385620914</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="18" customHeight="1">
-      <c r="B16" s="14" t="s">
+    <row r="16" spans="3:17" ht="18" customHeight="1">
+      <c r="C16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="15">
+      <c r="D16" s="10"/>
+      <c r="E16" s="12">
         <v>113</v>
       </c>
-      <c r="E16" s="15">
+      <c r="F16" s="12">
         <v>113</v>
       </c>
-      <c r="F16" s="15">
+      <c r="G16" s="12">
         <v>113</v>
       </c>
-      <c r="G16" s="15">
+      <c r="H16" s="12">
         <v>113</v>
       </c>
-      <c r="H16" s="15">
+      <c r="I16" s="12">
         <v>113</v>
       </c>
-      <c r="I16" s="15">
+      <c r="J16" s="12">
         <v>113</v>
       </c>
-      <c r="J16" s="15">
+      <c r="K16" s="12">
         <v>113</v>
       </c>
-      <c r="K16" s="15">
+      <c r="L16" s="12">
         <v>113</v>
       </c>
-      <c r="L16" s="15">
+      <c r="M16" s="12">
         <v>113</v>
       </c>
-      <c r="M16" s="15">
+      <c r="N16" s="12">
         <v>113</v>
       </c>
-      <c r="N16" s="19">
+      <c r="O16" s="16">
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-      <c r="O16" s="19">
+      <c r="P16" s="16">
         <f t="shared" si="1"/>
         <v>77.837168141592926</v>
       </c>
-      <c r="P16" s="20">
+      <c r="Q16" s="17">
         <f t="shared" si="2"/>
         <v>6.4864306784660775</v>
       </c>
     </row>
-    <row r="17" spans="2:16" ht="18" customHeight="1">
-      <c r="B17" s="14" t="s">
+    <row r="17" spans="3:17" ht="18" customHeight="1">
+      <c r="C17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="15">
+      <c r="E17" s="12">
         <v>106</v>
       </c>
-      <c r="E17" s="15">
+      <c r="F17" s="12">
         <v>105</v>
       </c>
-      <c r="F17" s="15">
+      <c r="G17" s="12">
         <v>105</v>
       </c>
-      <c r="G17" s="15">
+      <c r="H17" s="12">
         <v>106</v>
       </c>
-      <c r="H17" s="15">
+      <c r="I17" s="12">
         <v>105</v>
       </c>
-      <c r="I17" s="15">
+      <c r="J17" s="12">
         <v>107</v>
       </c>
-      <c r="J17" s="15">
+      <c r="K17" s="12">
         <v>106</v>
       </c>
-      <c r="K17" s="15">
+      <c r="L17" s="12">
         <v>105</v>
       </c>
-      <c r="L17" s="15">
+      <c r="M17" s="12">
         <v>106</v>
       </c>
-      <c r="M17" s="15">
+      <c r="N17" s="12">
         <v>105</v>
       </c>
-      <c r="N17" s="19">
+      <c r="O17" s="16">
         <f t="shared" si="0"/>
         <v>105.6</v>
       </c>
-      <c r="O17" s="19">
+      <c r="P17" s="16">
         <f t="shared" si="1"/>
         <v>83.291666666666671</v>
       </c>
-      <c r="P17" s="20">
+      <c r="Q17" s="17">
         <f t="shared" si="2"/>
         <v>6.9409722222222223</v>
       </c>
     </row>
-    <row r="18" spans="2:16" ht="18" customHeight="1" thickBot="1">
-      <c r="B18" s="34" t="s">
+    <row r="18" spans="3:17" ht="18" customHeight="1" thickBot="1">
+      <c r="C18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="D18" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="35">
+      <c r="E18" s="28">
         <v>103</v>
       </c>
-      <c r="E18" s="35">
+      <c r="F18" s="28">
         <v>102</v>
       </c>
-      <c r="F18" s="35">
+      <c r="G18" s="28">
         <v>102</v>
       </c>
-      <c r="G18" s="35">
+      <c r="H18" s="28">
         <v>102</v>
       </c>
-      <c r="H18" s="35">
+      <c r="I18" s="28">
         <v>102</v>
       </c>
-      <c r="I18" s="35">
+      <c r="J18" s="28">
         <v>102</v>
       </c>
-      <c r="J18" s="35">
+      <c r="K18" s="28">
         <v>102</v>
       </c>
-      <c r="K18" s="35">
+      <c r="L18" s="28">
         <v>102</v>
       </c>
-      <c r="L18" s="35">
+      <c r="M18" s="28">
         <v>102</v>
       </c>
-      <c r="M18" s="35">
+      <c r="N18" s="28">
         <v>102</v>
       </c>
-      <c r="N18" s="36">
+      <c r="O18" s="29">
         <f t="shared" si="0"/>
         <v>102.1</v>
       </c>
-      <c r="O18" s="36">
+      <c r="P18" s="29">
         <f t="shared" si="1"/>
         <v>86.146914789422141</v>
       </c>
-      <c r="P18" s="37">
+      <c r="Q18" s="30">
         <f t="shared" si="2"/>
         <v>7.1789095657851787</v>
       </c>
     </row>
-    <row r="19" spans="2:16" ht="16" thickTop="1"/>
+    <row r="19" spans="3:17" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="O10:O11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>